<commit_message>
WIP prototyping the lookup functions
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>ca</t>
   </si>
@@ -95,10 +95,55 @@
     <t>A</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>MAX</t>
   </si>
   <si>
     <t>MIN</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>LOOKUP</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>HLOOKUP</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>RADIANS</t>
@@ -459,9 +504,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD66"/>
     </sheetView>
   </sheetViews>
@@ -1657,7 +1702,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>-10</v>
@@ -1681,7 +1726,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>-10</v>
@@ -1705,7 +1750,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B45">
         <f>PI()</f>
@@ -1748,7 +1793,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B46">
         <v>120</v>
@@ -1789,7 +1834,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -1833,7 +1878,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B48">
         <v>31.5</v>
@@ -1877,7 +1922,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -1919,40 +1964,337 @@
         <v>6.2850422557600663</v>
       </c>
     </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" t="s">
+        <v>29</v>
+      </c>
+      <c r="I51" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>0.7378690916947479</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="2">
+        <f>LOOKUP(E52,$A$52:$A$59,$C$52:$C$59)</f>
+        <v>0.47907823066425825</v>
+      </c>
+      <c r="G52">
+        <f>MATCH(E52,$A$52:$A$59,1)</f>
+        <v>2</v>
+      </c>
+      <c r="H52" s="2">
+        <f>VLOOKUP(E52,$A$52:$C$59,2)</f>
+        <v>4</v>
+      </c>
+      <c r="I52" t="str">
+        <f>HLOOKUP(D52,$A$62:$E$63,2,TRUE)</f>
+        <v>D</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>0.47907823066425825</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="2">
+        <f>LOOKUP(E53,$A$52:$A$59,$C$52:$C$59)</f>
+        <v>3.0309719327287099E-2</v>
+      </c>
+      <c r="G53">
+        <f>MATCH(E53,$A$52:$A$59,1)</f>
+        <v>4</v>
+      </c>
+      <c r="H53" s="2">
+        <f>VLOOKUP(E53,$A$52:$C$59,2)</f>
+        <v>7</v>
+      </c>
+      <c r="I53" t="e">
+        <f>HLOOKUP(D53,$A$62:$E$63,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F54" s="2"/>
-      <c r="H54" s="2"/>
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0.96857495724960163</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="2">
+        <f>LOOKUP(E54,$A$52:$A$59,$C$52:$C$59)</f>
+        <v>0.53897460771383143</v>
+      </c>
+      <c r="G54">
+        <f>MATCH(H54,$B$52:$B$59,1)</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="2">
+        <f>VLOOKUP(E54,$A$52:$C$59,2)</f>
+        <v>3</v>
+      </c>
+      <c r="I54" t="e">
+        <f>HLOOKUP(E54,$A$63:$E$64,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K54">
+        <f ca="1">SUMIF(B52:B59,"&gt;6",C52:C58)</f>
+        <v>3.0309719327287099E-2</v>
+      </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="A55" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>3.0309719327287099E-2</v>
+      </c>
+      <c r="D55">
+        <v>5</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="2">
+        <f>LOOKUP(E55,$A$52:$A$59,$C$52:$C$59)</f>
+        <v>0.96857495724960163</v>
+      </c>
+      <c r="G55">
+        <f>MATCH(E55,$A$52:$A$59,1)</f>
+        <v>3</v>
+      </c>
+      <c r="H55" s="2">
+        <f>VLOOKUP(E55,$A$52:$C$59,3)</f>
+        <v>0.96857495724960163</v>
+      </c>
+      <c r="I55">
+        <f>HLOOKUP(E55,$A$63:$E$64,2,FALSE)</f>
+        <v>234</v>
+      </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>0.35204476099741322</v>
+      </c>
+      <c r="D56">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="2" t="e">
+        <f>LOOKUP(E56,$B$52:$B$59,$C$52:$C$59)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G56">
+        <f>MATCH(B57,$B$52:$B$59,1)</f>
+        <v>6</v>
+      </c>
+      <c r="H56" s="2">
+        <f>VLOOKUP(E56,$A$52:$C$59,2)</f>
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <f>HLOOKUP(D56,$A$62:$E$64,3,TRUE)</f>
+        <v>54</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57" s="2">
+        <f>LOOKUP(E57,$B$52:$B$59,$C$52:$C$59)</f>
+        <v>3.0309719327287099E-2</v>
+      </c>
+      <c r="G57">
+        <f>MATCH(5.5,$D$52:$D$59,-1)</f>
+        <v>3</v>
+      </c>
+      <c r="H57" s="2">
+        <f>VLOOKUP(E57,$B$52:$C$59,2)</f>
+        <v>3.0309719327287099E-2</v>
+      </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F58" s="2"/>
-      <c r="H58" s="2"/>
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+      <c r="C58">
+        <v>0.20954842656952388</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" s="2" t="e">
+        <f>LOOKUP(E58,$B$52:$B$59,$C$52:$C$59)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G58" t="e">
+        <f>MATCH(E58,$A$52:$A$59,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H58" s="2">
+        <f>VLOOKUP(E58,$A$52:$C$59,2)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H59" s="2"/>
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>0.53897460771383143</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59">
+        <f>MATCH(5.5,$D$52:$D$59,-5)</f>
+        <v>3</v>
+      </c>
+      <c r="H59" s="2">
+        <f>VLOOKUP(E59,$A$52:$C$59,2)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H60" s="2"/>
+      <c r="E60" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="2">
+        <f>VLOOKUP(E60,$A$52:$C$59,2,FALSE)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <f t="array" ref="H61">SUM(VLOOKUP(A58:A59,$A$52:$C$59,3,FALSE))</f>
+        <v>0.20954842656952388</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>55</v>
+      </c>
+      <c r="B64">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>54</v>
+      </c>
+      <c r="D64">
+        <v>234</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WIP updated lookup function and test.xlsx
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:U65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2567,6 +2567,10 @@
       <c r="E60" t="s">
         <v>36</v>
       </c>
+      <c r="F60">
+        <f>LOOKUP(E58,$B$53:$B$60,$C$53:$C$60)</f>
+        <v>3.0309719327287099E-2</v>
+      </c>
       <c r="G60">
         <f>MATCH(5.5,$D$52:$D$59,-5)</f>
         <v>4</v>
@@ -2579,6 +2583,10 @@
     <row r="61" spans="1:19">
       <c r="E61" t="s">
         <v>36</v>
+      </c>
+      <c r="F61">
+        <f>LOOKUP(E56,$A$53:$A$60,$C$53:$C$60)</f>
+        <v>0.96857495724960163</v>
       </c>
       <c r="H61" s="2">
         <f>VLOOKUP(E61,$A$52:$C$59,2,FALSE)</f>

</xml_diff>